<commit_message>
fix path for figs
</commit_message>
<xml_diff>
--- a/src/UM5MES02.xlsx
+++ b/src/UM5MES02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maurini/Cloud/drop-su/Enseignement/master/fichesUE/master-mecanique/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77A55CB-00AB-9E40-BF42-92BE07C24C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A695D97-71DC-B345-893E-B08BF096600A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11560" yWindow="2860" windowWidth="38400" windowHeight="21100" xr2:uid="{946D5765-8A67-8240-B7B5-AEFFB1FB0322}"/>
   </bookViews>
@@ -293,7 +293,7 @@
     <t>Nom de fichier pour une image</t>
   </si>
   <si>
-    <t>UM5MES02-fig.pdf</t>
+    <t>UM5MES02-fig.png</t>
   </si>
 </sst>
 </file>
@@ -730,7 +730,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>